<commit_message>
dynamic loss is ready
</commit_message>
<xml_diff>
--- a/attributes/common attributes.xlsx
+++ b/attributes/common attributes.xlsx
@@ -20,14 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="137">
+  <si>
+    <t xml:space="preserve">CA_Duke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA100k</t>
+  </si>
   <si>
     <t xml:space="preserve">CA_Market</t>
   </si>
   <si>
-    <t xml:space="preserve">PA100k</t>
-  </si>
-  <si>
     <t xml:space="preserve">gender</t>
   </si>
   <si>
@@ -40,7 +43,13 @@
     <t xml:space="preserve">AgeOver60</t>
   </si>
   <si>
-    <t xml:space="preserve">11, 12,13</t>
+    <t xml:space="preserve">10, 11,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cap</t>
   </si>
   <si>
     <t xml:space="preserve">short hair</t>
@@ -49,40 +58,70 @@
     <t xml:space="preserve">Age18-60</t>
   </si>
   <si>
+    <t xml:space="preserve">Glasses</t>
+  </si>
+  <si>
     <t xml:space="preserve">longhair(straight)</t>
   </si>
   <si>
     <t xml:space="preserve">AgeLess18</t>
   </si>
   <si>
+    <t xml:space="preserve">bag</t>
+  </si>
+  <si>
     <t xml:space="preserve">knot</t>
   </si>
   <si>
     <t xml:space="preserve">Front</t>
   </si>
   <si>
+    <t xml:space="preserve">LongCoat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long hair</t>
+  </si>
+  <si>
     <t xml:space="preserve">unvisible(hair)</t>
   </si>
   <si>
     <t xml:space="preserve">Side</t>
   </si>
   <si>
+    <t xml:space="preserve">pants</t>
+  </si>
+  <si>
     <t xml:space="preserve">burnette</t>
   </si>
   <si>
     <t xml:space="preserve">Back</t>
   </si>
   <si>
+    <t xml:space="preserve">shorts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h_colorful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">blonde</t>
   </si>
   <si>
-    <t xml:space="preserve">Hat</t>
+    <t xml:space="preserve">skirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h_black</t>
   </si>
   <si>
     <t xml:space="preserve">black</t>
   </si>
   <si>
-    <t xml:space="preserve">Glasses</t>
+    <t xml:space="preserve">boots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tshirt_shs</t>
   </si>
   <si>
     <t xml:space="preserve">no-color</t>
@@ -91,16 +130,22 @@
     <t xml:space="preserve">HandBag</t>
   </si>
   <si>
-    <t xml:space="preserve">cap</t>
+    <t xml:space="preserve">Backpack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shirt_ls</t>
   </si>
   <si>
     <t xml:space="preserve">ShoulderBag</t>
   </si>
   <si>
+    <t xml:space="preserve">coat</t>
+  </si>
+  <si>
     <t xml:space="preserve">snowcap</t>
   </si>
   <si>
-    <t xml:space="preserve">Backpack</t>
+    <t xml:space="preserve">top</t>
   </si>
   <si>
     <t xml:space="preserve">hoodiecap</t>
@@ -109,58 +154,85 @@
     <t xml:space="preserve">HoldObjectsInFront</t>
   </si>
   <si>
+    <t xml:space="preserve">simple/patterned</t>
+  </si>
+  <si>
     <t xml:space="preserve">no cap</t>
   </si>
   <si>
     <t xml:space="preserve">ShortSleeve</t>
   </si>
   <si>
+    <t xml:space="preserve">b_w</t>
+  </si>
+  <si>
     <t xml:space="preserve">unvisible(cap)</t>
   </si>
   <si>
     <t xml:space="preserve">LongSleeve</t>
   </si>
   <si>
+    <t xml:space="preserve">b_r</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_white</t>
   </si>
   <si>
     <t xml:space="preserve">UpperStride</t>
   </si>
   <si>
+    <t xml:space="preserve">b_y</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_blue</t>
   </si>
   <si>
     <t xml:space="preserve">UpperLogo</t>
   </si>
   <si>
+    <t xml:space="preserve">b_green</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_green</t>
   </si>
   <si>
     <t xml:space="preserve">UpperPlaid</t>
   </si>
   <si>
+    <t xml:space="preserve">b_b</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_red</t>
   </si>
   <si>
     <t xml:space="preserve">UpperSplice</t>
   </si>
   <si>
+    <t xml:space="preserve">b_gray</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_brown</t>
   </si>
   <si>
     <t xml:space="preserve">LowerStripe</t>
   </si>
   <si>
+    <t xml:space="preserve">b_p</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_yellow</t>
   </si>
   <si>
     <t xml:space="preserve">LowerPattern</t>
   </si>
   <si>
+    <t xml:space="preserve">b_black</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_gray</t>
   </si>
   <si>
-    <t xml:space="preserve">LongCoat</t>
+    <t xml:space="preserve">backpack</t>
   </si>
   <si>
     <t xml:space="preserve">c_black</t>
@@ -169,91 +241,136 @@
     <t xml:space="preserve">Trousers</t>
   </si>
   <si>
+    <t xml:space="preserve">shoulder bag</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shorts</t>
   </si>
   <si>
+    <t xml:space="preserve">hand bag</t>
+  </si>
+  <si>
     <t xml:space="preserve">T-shirt/shirt</t>
   </si>
   <si>
     <t xml:space="preserve">Skirt&amp;Dress</t>
   </si>
   <si>
+    <t xml:space="preserve">no bag</t>
+  </si>
+  <si>
     <t xml:space="preserve">jacket/sweatshirt</t>
   </si>
   <si>
-    <t xml:space="preserve">boots</t>
-  </si>
-  <si>
     <t xml:space="preserve">overcoat</t>
   </si>
   <si>
+    <t xml:space="preserve">short</t>
+  </si>
+  <si>
     <t xml:space="preserve">hoodie</t>
   </si>
   <si>
     <t xml:space="preserve">b_white</t>
   </si>
   <si>
+    <t xml:space="preserve">l_w</t>
+  </si>
+  <si>
     <t xml:space="preserve">b_purple</t>
   </si>
   <si>
+    <t xml:space="preserve">l_r</t>
+  </si>
+  <si>
     <t xml:space="preserve">b_pink</t>
   </si>
   <si>
+    <t xml:space="preserve">l_br</t>
+  </si>
+  <si>
     <t xml:space="preserve">b_blue</t>
   </si>
   <si>
-    <t xml:space="preserve">b_green</t>
+    <t xml:space="preserve">l_y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l_green</t>
   </si>
   <si>
     <t xml:space="preserve">b_red</t>
   </si>
   <si>
+    <t xml:space="preserve">l_b</t>
+  </si>
+  <si>
     <t xml:space="preserve">b_brown</t>
   </si>
   <si>
+    <t xml:space="preserve">l_gray</t>
+  </si>
+  <si>
     <t xml:space="preserve">b_yellow</t>
   </si>
   <si>
-    <t xml:space="preserve">b_gray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b_black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backpack</t>
+    <t xml:space="preserve">l_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l_black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandal</t>
   </si>
   <si>
     <t xml:space="preserve">bag/handbag</t>
   </si>
   <si>
+    <t xml:space="preserve">hidden</t>
+  </si>
+  <si>
     <t xml:space="preserve">no bags</t>
   </si>
   <si>
+    <t xml:space="preserve">no color</t>
+  </si>
+  <si>
     <t xml:space="preserve">umbrella(open)</t>
   </si>
   <si>
+    <t xml:space="preserve">f_w</t>
+  </si>
+  <si>
     <t xml:space="preserve">umbrella(closed)</t>
   </si>
   <si>
+    <t xml:space="preserve">f_colorful</t>
+  </si>
+  <si>
     <t xml:space="preserve">no umbrella</t>
   </si>
   <si>
+    <t xml:space="preserve">f_black</t>
+  </si>
+  <si>
     <t xml:space="preserve">beard</t>
   </si>
   <si>
+    <t xml:space="preserve">young</t>
+  </si>
+  <si>
     <t xml:space="preserve">shaved</t>
   </si>
   <si>
-    <t xml:space="preserve">hidden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shorts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skirt</t>
+    <t xml:space="preserve">teenager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">old</t>
   </si>
   <si>
     <t xml:space="preserve">unvisible</t>
@@ -265,9 +382,6 @@
     <t xml:space="preserve">l_blue</t>
   </si>
   <si>
-    <t xml:space="preserve">l_green</t>
-  </si>
-  <si>
     <t xml:space="preserve">l_red</t>
   </si>
   <si>
@@ -277,12 +391,6 @@
     <t xml:space="preserve">l_yellow</t>
   </si>
   <si>
-    <t xml:space="preserve">l_gray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_black</t>
-  </si>
-  <si>
     <t xml:space="preserve">formal shoes</t>
   </si>
   <si>
@@ -295,16 +403,10 @@
     <t xml:space="preserve">f_white</t>
   </si>
   <si>
-    <t xml:space="preserve">f_colorful</t>
-  </si>
-  <si>
     <t xml:space="preserve">f_brown</t>
   </si>
   <si>
     <t xml:space="preserve">f_gray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f_black</t>
   </si>
   <si>
     <t xml:space="preserve">sunglasses</t>
@@ -442,10 +544,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,7 +555,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,852 +575,1759 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>1</v>
+      <c r="J2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>8</v>
+      <c r="L3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>9</v>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>10.11</v>
+      <c r="O5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="n">
+      <c r="F9" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>25</v>
+      <c r="P9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="P10" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>61</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>64</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>80</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>82</v>
+      </c>
+      <c r="J29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>83</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
+        <v>85</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>58</v>
+        <v>87</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
+        <v>92</v>
+      </c>
+      <c r="J35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>62</v>
+        <v>94</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>67</v>
+        <v>101</v>
+      </c>
+      <c r="J41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>103</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>105</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>107</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>109</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>72</v>
+        <v>111</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>73</v>
+        <v>113</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>102</v>
+      </c>
+      <c r="J48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>75</v>
+        <v>22</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>76</v>
+        <v>25</v>
+      </c>
+      <c r="J50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>77</v>
+        <v>29</v>
+      </c>
+      <c r="J51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>78</v>
+        <v>117</v>
+      </c>
+      <c r="J52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>79</v>
+        <v>118</v>
+      </c>
+      <c r="J53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>80</v>
+        <v>119</v>
+      </c>
+      <c r="J54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
+      </c>
+      <c r="J55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
+      </c>
+      <c r="J56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>83</v>
+        <v>121</v>
+      </c>
+      <c r="J57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>84</v>
+        <v>122</v>
+      </c>
+      <c r="J58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
+      </c>
+      <c r="J59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
+      </c>
+      <c r="J60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="J61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>87</v>
+        <v>123</v>
+      </c>
+      <c r="J62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>88</v>
+        <v>124</v>
+      </c>
+      <c r="J63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>89</v>
+        <v>125</v>
+      </c>
+      <c r="J64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>74</v>
+        <v>102</v>
+      </c>
+      <c r="J65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>90</v>
+        <v>126</v>
+      </c>
+      <c r="J66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
+      </c>
+      <c r="J67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>92</v>
+        <v>127</v>
+      </c>
+      <c r="J68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>93</v>
+        <v>128</v>
+      </c>
+      <c r="J69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>94</v>
+        <v>110</v>
+      </c>
+      <c r="J70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="J71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>95</v>
+        <v>129</v>
+      </c>
+      <c r="J72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>96</v>
+        <v>130</v>
+      </c>
+      <c r="J73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>97</v>
+        <v>131</v>
+      </c>
+      <c r="J74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>98</v>
+        <v>132</v>
+      </c>
+      <c r="J75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>99</v>
+        <v>133</v>
+      </c>
+      <c r="J76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>100</v>
+        <v>134</v>
+      </c>
+      <c r="J77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>101</v>
+        <v>135</v>
+      </c>
+      <c r="J78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="J79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>102</v>
+        <v>136</v>
+      </c>
+      <c r="J80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dynamic loss weighting modified
</commit_message>
<xml_diff>
--- a/attributes/common attributes.xlsx
+++ b/attributes/common attributes.xlsx
@@ -445,6 +445,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -466,6 +467,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -547,10 +549,10 @@
   <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
@@ -558,7 +560,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
a function for plotting from a list is added
</commit_message>
<xml_diff>
--- a/attributes/common attributes.xlsx
+++ b/attributes/common attributes.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="147">
   <si>
     <t xml:space="preserve">CA_Duke</t>
   </si>
@@ -28,9 +28,27 @@
     <t xml:space="preserve">PA100k</t>
   </si>
   <si>
+    <t xml:space="preserve">common</t>
+  </si>
+  <si>
+    <t xml:space="preserve">index</t>
+  </si>
+  <si>
     <t xml:space="preserve">CA_Market</t>
   </si>
   <si>
+    <t xml:space="preserve">CA_Duke_Market</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDM_idx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA_idx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commons</t>
+  </si>
+  <si>
     <t xml:space="preserve">gender</t>
   </si>
   <si>
@@ -61,6 +79,9 @@
     <t xml:space="preserve">Glasses</t>
   </si>
   <si>
+    <t xml:space="preserve">ShoulderBag</t>
+  </si>
+  <si>
     <t xml:space="preserve">longhair(straight)</t>
   </si>
   <si>
@@ -70,6 +91,9 @@
     <t xml:space="preserve">bag</t>
   </si>
   <si>
+    <t xml:space="preserve">Backpack</t>
+  </si>
+  <si>
     <t xml:space="preserve">knot</t>
   </si>
   <si>
@@ -82,13 +106,16 @@
     <t xml:space="preserve">long hair</t>
   </si>
   <si>
+    <t xml:space="preserve">pants</t>
+  </si>
+  <si>
     <t xml:space="preserve">unvisible(hair)</t>
   </si>
   <si>
     <t xml:space="preserve">Side</t>
   </si>
   <si>
-    <t xml:space="preserve">pants</t>
+    <t xml:space="preserve">shorts</t>
   </si>
   <si>
     <t xml:space="preserve">burnette</t>
@@ -97,24 +124,24 @@
     <t xml:space="preserve">Back</t>
   </si>
   <si>
-    <t xml:space="preserve">shorts</t>
-  </si>
-  <si>
     <t xml:space="preserve">h_colorful</t>
   </si>
   <si>
-    <t xml:space="preserve">6,7</t>
+    <t xml:space="preserve">6,7,15:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skirt</t>
   </si>
   <si>
     <t xml:space="preserve">blonde</t>
   </si>
   <si>
-    <t xml:space="preserve">skirt</t>
-  </si>
-  <si>
     <t xml:space="preserve">h_black</t>
   </si>
   <si>
+    <t xml:space="preserve">8,22</t>
+  </si>
+  <si>
     <t xml:space="preserve">black</t>
   </si>
   <si>
@@ -124,30 +151,36 @@
     <t xml:space="preserve">Tshirt_shs</t>
   </si>
   <si>
+    <t xml:space="preserve">b_white</t>
+  </si>
+  <si>
     <t xml:space="preserve">no-color</t>
   </si>
   <si>
     <t xml:space="preserve">HandBag</t>
   </si>
   <si>
-    <t xml:space="preserve">Backpack</t>
-  </si>
-  <si>
     <t xml:space="preserve">shirt_ls</t>
   </si>
   <si>
-    <t xml:space="preserve">ShoulderBag</t>
+    <t xml:space="preserve">b_red</t>
   </si>
   <si>
     <t xml:space="preserve">coat</t>
   </si>
   <si>
+    <t xml:space="preserve">b_yellow</t>
+  </si>
+  <si>
     <t xml:space="preserve">snowcap</t>
   </si>
   <si>
     <t xml:space="preserve">top</t>
   </si>
   <si>
+    <t xml:space="preserve">b_green</t>
+  </si>
+  <si>
     <t xml:space="preserve">hoodiecap</t>
   </si>
   <si>
@@ -157,6 +190,9 @@
     <t xml:space="preserve">simple/patterned</t>
   </si>
   <si>
+    <t xml:space="preserve">b_blue</t>
+  </si>
+  <si>
     <t xml:space="preserve">no cap</t>
   </si>
   <si>
@@ -166,6 +202,9 @@
     <t xml:space="preserve">b_w</t>
   </si>
   <si>
+    <t xml:space="preserve">b_gray</t>
+  </si>
+  <si>
     <t xml:space="preserve">unvisible(cap)</t>
   </si>
   <si>
@@ -175,6 +214,9 @@
     <t xml:space="preserve">b_r</t>
   </si>
   <si>
+    <t xml:space="preserve">b_purple</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_white</t>
   </si>
   <si>
@@ -184,13 +226,16 @@
     <t xml:space="preserve">b_y</t>
   </si>
   <si>
+    <t xml:space="preserve">b_black</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_blue</t>
   </si>
   <si>
     <t xml:space="preserve">UpperLogo</t>
   </si>
   <si>
-    <t xml:space="preserve">b_green</t>
+    <t xml:space="preserve">backpack</t>
   </si>
   <si>
     <t xml:space="preserve">c_green</t>
@@ -202,13 +247,19 @@
     <t xml:space="preserve">b_b</t>
   </si>
   <si>
+    <t xml:space="preserve">22,23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hand bag</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_red</t>
   </si>
   <si>
     <t xml:space="preserve">UpperSplice</t>
   </si>
   <si>
-    <t xml:space="preserve">b_gray</t>
+    <t xml:space="preserve">no bag</t>
   </si>
   <si>
     <t xml:space="preserve">c_brown</t>
@@ -226,15 +277,12 @@
     <t xml:space="preserve">LowerPattern</t>
   </si>
   <si>
-    <t xml:space="preserve">b_black</t>
+    <t xml:space="preserve">short</t>
   </si>
   <si>
     <t xml:space="preserve">c_gray</t>
   </si>
   <si>
-    <t xml:space="preserve">backpack</t>
-  </si>
-  <si>
     <t xml:space="preserve">c_black</t>
   </si>
   <si>
@@ -244,10 +292,13 @@
     <t xml:space="preserve">shoulder bag</t>
   </si>
   <si>
+    <t xml:space="preserve">l_w</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shorts</t>
   </si>
   <si>
-    <t xml:space="preserve">hand bag</t>
+    <t xml:space="preserve">l_r</t>
   </si>
   <si>
     <t xml:space="preserve">T-shirt/shirt</t>
@@ -256,70 +307,64 @@
     <t xml:space="preserve">Skirt&amp;Dress</t>
   </si>
   <si>
-    <t xml:space="preserve">no bag</t>
+    <t xml:space="preserve">l_br</t>
   </si>
   <si>
     <t xml:space="preserve">jacket/sweatshirt</t>
   </si>
   <si>
+    <t xml:space="preserve">l_y</t>
+  </si>
+  <si>
     <t xml:space="preserve">overcoat</t>
   </si>
   <si>
-    <t xml:space="preserve">short</t>
+    <t xml:space="preserve">l_green</t>
   </si>
   <si>
     <t xml:space="preserve">hoodie</t>
   </si>
   <si>
-    <t xml:space="preserve">b_white</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_w</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b_purple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_r</t>
+    <t xml:space="preserve">l_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l_gray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l_p</t>
   </si>
   <si>
     <t xml:space="preserve">b_pink</t>
   </si>
   <si>
-    <t xml:space="preserve">l_br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b_blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b_red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_b</t>
+    <t xml:space="preserve">l_black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,61,62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no color</t>
   </si>
   <si>
     <t xml:space="preserve">b_brown</t>
   </si>
   <si>
-    <t xml:space="preserve">l_gray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b_yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l_black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shoes</t>
+    <t xml:space="preserve">f_w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65,66,67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_colorful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_black</t>
   </si>
   <si>
     <t xml:space="preserve">sandal</t>
@@ -328,31 +373,16 @@
     <t xml:space="preserve">bag/handbag</t>
   </si>
   <si>
-    <t xml:space="preserve">hidden</t>
-  </si>
-  <si>
     <t xml:space="preserve">no bags</t>
   </si>
   <si>
-    <t xml:space="preserve">no color</t>
-  </si>
-  <si>
     <t xml:space="preserve">umbrella(open)</t>
   </si>
   <si>
-    <t xml:space="preserve">f_w</t>
-  </si>
-  <si>
     <t xml:space="preserve">umbrella(closed)</t>
   </si>
   <si>
-    <t xml:space="preserve">f_colorful</t>
-  </si>
-  <si>
     <t xml:space="preserve">no umbrella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f_black</t>
   </si>
   <si>
     <t xml:space="preserve">beard</t>
@@ -546,21 +576,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC28" activeCellId="0" sqref="AC28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="26" style="1" width="8.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,38 +619,71 @@
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>0</v>
@@ -622,28 +692,56 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="1" t="n">
+      <c r="K2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="1" t="n">
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>3</v>
+      <c r="Q2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,43 +749,71 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="1" t="n">
+      <c r="K3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="P3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>9</v>
+      <c r="AA3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,13 +821,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>70</v>
@@ -710,28 +836,56 @@
         <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="Z4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="L4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>5</v>
+      <c r="AA4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,13 +893,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>39</v>
@@ -754,28 +908,56 @@
         <v>9.1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="1" t="n">
+      <c r="K5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="1" t="n">
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="P5" s="1" t="n">
+      <c r="Q5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>10</v>
+      <c r="R5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,13 +965,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>26</v>
@@ -798,28 +980,56 @@
         <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="1" t="n">
+      <c r="K6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y6" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="O6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>19</v>
+      <c r="Z6" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,13 +1037,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>47</v>
@@ -842,28 +1052,56 @@
         <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y7" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="L7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>16</v>
+      <c r="Z7" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,13 +1109,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>48</v>
@@ -886,28 +1124,56 @@
         <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="1" t="n">
+      <c r="K8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="1" t="n">
+      <c r="L8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>26</v>
+      <c r="N8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="Z8" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,13 +1181,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>49</v>
@@ -930,28 +1196,47 @@
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="I9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="1" t="n">
+      <c r="K9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="P9" s="1" t="n">
+      <c r="L9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>30</v>
+      <c r="N9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,13 +1244,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>62</v>
@@ -974,28 +1259,47 @@
         <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="I10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="1" t="n">
+      <c r="K10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="1" t="n">
-        <v>62</v>
+      <c r="L10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P10" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="Q10" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,13 +1307,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>38</v>
@@ -1018,28 +1322,47 @@
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="1" t="n">
+      <c r="K11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O11" s="1" t="n">
-        <v>38</v>
+      <c r="L11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,25 +1370,50 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="K12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="1" t="n">
+      <c r="L12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>39</v>
+      <c r="N12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,25 +1421,50 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="K13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="1" t="n">
+      <c r="L13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>41</v>
+      <c r="N13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,25 +1472,50 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="K14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="1" t="n">
+      <c r="L14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>44</v>
+      <c r="N14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,25 +1523,50 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="K15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L15" s="1" t="n">
+      <c r="L15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>47</v>
+      <c r="N15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P15" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,25 +1574,50 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="K16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L16" s="1" t="n">
+      <c r="L16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>50</v>
+      <c r="N16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,25 +1625,50 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="K17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L17" s="1" t="n">
+      <c r="L17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>53</v>
+      <c r="N17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,25 +1676,50 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="K18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L18" s="1" t="n">
+      <c r="L18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>56</v>
+      <c r="N18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P18" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="Q18" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,25 +1727,50 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="K19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L19" s="1" t="n">
+      <c r="L19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>59</v>
+      <c r="N19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="W19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,25 +1778,50 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="K20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L20" s="1" t="n">
+      <c r="P20" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>62</v>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,25 +1829,50 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="K21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L21" s="1" t="n">
+      <c r="L21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>65</v>
+      <c r="N21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P21" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,25 +1880,50 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="K22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L22" s="1" t="n">
+      <c r="L22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>68</v>
+      </c>
+      <c r="P22" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="Q22" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,25 +1931,50 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="K23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L23" s="1" t="n">
+      <c r="L23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>70</v>
+      <c r="N23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P23" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="Q23" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,25 +1982,50 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J24" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="K24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L24" s="1" t="n">
+      <c r="L24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>73</v>
+      <c r="N24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P24" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="Q24" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,25 +2033,50 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="K25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L25" s="1" t="n">
+      <c r="L25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>75</v>
+      <c r="N25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P25" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="Q25" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="S25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,25 +2084,50 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J26" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="K26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L26" s="1" t="n">
+      <c r="L26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>78</v>
+      <c r="N26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P26" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q26" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="W26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1437,25 +2135,50 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="K27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L27" s="1" t="n">
+      <c r="L27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>22</v>
+      <c r="N27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P27" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,19 +2186,38 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="K28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L28" s="1" t="n">
+      <c r="L28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>81</v>
+      <c r="N28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P28" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,19 +2225,38 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J29" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L29" s="1" t="n">
+      <c r="L29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>29</v>
+      <c r="N29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P29" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="Q29" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,19 +2264,38 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J30" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="K30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L30" s="1" t="n">
+      <c r="L30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>84</v>
+      <c r="N30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P30" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="Q30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,19 +2303,38 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J31" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="K31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L31" s="1" t="n">
+      <c r="L31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>86</v>
+      <c r="N31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="S31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,19 +2342,38 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J32" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="K32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L32" s="1" t="n">
+      <c r="L32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>88</v>
+      <c r="N32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P32" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="Q32" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,19 +2381,38 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J33" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="K33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L33" s="1" t="n">
+      <c r="L33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>90</v>
+      <c r="N33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="S33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,19 +2420,38 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J34" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="K34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L34" s="1" t="n">
+      <c r="L34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>91</v>
+      <c r="N34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P34" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q34" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,19 +2459,38 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J35" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="K35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L35" s="1" t="n">
+      <c r="L35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>93</v>
+      <c r="N35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P35" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,19 +2498,38 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J36" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="K36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L36" s="1" t="n">
+      <c r="L36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>95</v>
+      <c r="N36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P36" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="Q36" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,19 +2537,38 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J37" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="K37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L37" s="1" t="n">
+      <c r="L37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="M37" s="1" t="s">
-        <v>97</v>
+      <c r="N37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q37" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="S37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,19 +2576,38 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J38" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="K38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L38" s="1" t="n">
+      <c r="L38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>98</v>
+      <c r="N38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="S38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,17 +2617,17 @@
       <c r="B39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J39" s="1" t="n">
+      <c r="K39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L39" s="1" t="n">
+      <c r="M39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>99</v>
+      <c r="N39" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,19 +2635,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J40" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="K40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L40" s="1" t="n">
+      <c r="L40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>100</v>
+      <c r="N40" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1723,19 +2655,19 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J41" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="K41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L41" s="1" t="n">
+      <c r="L41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>102</v>
+      <c r="N41" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,19 +2675,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J42" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="K42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L42" s="1" t="n">
+      <c r="L42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>104</v>
+      <c r="N42" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,19 +2695,19 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J43" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="K43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L43" s="1" t="n">
+      <c r="L43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>106</v>
+      <c r="N43" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,19 +2715,19 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J44" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="K44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="K44" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L44" s="1" t="n">
+      <c r="L44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="M44" s="1" t="s">
-        <v>108</v>
+      <c r="N44" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,19 +2735,19 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J45" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="K45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L45" s="1" t="n">
+      <c r="L45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="M45" s="1" t="s">
-        <v>110</v>
+      <c r="N45" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,19 +2755,19 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J46" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="K46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="K46" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L46" s="1" t="n">
+      <c r="L46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="M46" s="1" t="s">
-        <v>112</v>
+      <c r="N46" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1843,19 +2775,19 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J47" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="K47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L47" s="1" t="n">
+      <c r="L47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="M47" s="1" t="s">
-        <v>114</v>
+      <c r="N47" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,19 +2795,19 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J48" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="K48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L48" s="1" t="n">
+      <c r="L48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="M48" s="1" t="s">
-        <v>115</v>
+      <c r="N48" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,19 +2815,19 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J49" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="K49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L49" s="1" t="n">
+      <c r="L49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>116</v>
+      <c r="N49" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,13 +2835,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J50" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="K50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>25</v>
+      <c r="L50" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,13 +2849,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J51" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="K51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>29</v>
+      <c r="L51" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,13 +2863,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J52" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="K52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>117</v>
+      <c r="L52" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,13 +2877,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J53" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="K53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>118</v>
+      <c r="L53" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1959,13 +2891,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J54" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="K54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>119</v>
+      <c r="L54" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,13 +2905,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J55" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="K55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="K55" s="1" t="s">
-        <v>91</v>
+      <c r="L55" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,13 +2919,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J56" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="K56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="K56" s="1" t="s">
-        <v>120</v>
+      <c r="L56" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2001,13 +2933,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J57" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="K57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="K57" s="1" t="s">
-        <v>121</v>
+      <c r="L57" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,13 +2947,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J58" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="K58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="K58" s="1" t="s">
-        <v>122</v>
+      <c r="L58" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,13 +2961,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J59" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="K59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="K59" s="1" t="s">
-        <v>95</v>
+      <c r="L59" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,13 +2975,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J60" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="K60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="K60" s="1" t="s">
-        <v>98</v>
+      <c r="L60" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,13 +2989,13 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J61" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="K61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>34</v>
+      <c r="L61" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,13 +3003,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J62" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="K62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="K62" s="1" t="s">
-        <v>123</v>
+      <c r="L62" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2085,13 +3017,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J63" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="K63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="K63" s="1" t="s">
-        <v>124</v>
+      <c r="L63" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2099,13 +3031,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J64" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="K64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="K64" s="1" t="s">
-        <v>125</v>
+      <c r="L64" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,13 +3045,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J65" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="K65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="K65" s="1" t="s">
-        <v>102</v>
+      <c r="L65" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,13 +3059,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J66" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="K66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="K66" s="1" t="s">
-        <v>126</v>
+      <c r="L66" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,13 +3073,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J67" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="K67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="K67" s="1" t="s">
-        <v>108</v>
+      <c r="L67" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,13 +3087,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J68" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="K68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="K68" s="1" t="s">
-        <v>127</v>
+      <c r="L68" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,13 +3101,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J69" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="K69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="K69" s="1" t="s">
-        <v>128</v>
+      <c r="L69" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,13 +3115,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J70" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="K70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="K70" s="1" t="s">
-        <v>110</v>
+      <c r="L70" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,13 +3129,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J71" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="K71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="K71" s="1" t="s">
-        <v>34</v>
+      <c r="L71" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,13 +3143,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J72" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="K72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="K72" s="1" t="s">
-        <v>129</v>
+      <c r="L72" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,13 +3157,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J73" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="K73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="K73" s="1" t="s">
-        <v>130</v>
+      <c r="L73" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,13 +3171,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J74" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="K74" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="K74" s="1" t="s">
-        <v>131</v>
+      <c r="L74" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,13 +3185,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J75" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="K75" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>132</v>
+      <c r="L75" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,13 +3199,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="J76" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="K76" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="K76" s="1" t="s">
-        <v>133</v>
+      <c r="L76" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,13 +3213,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J77" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="K77" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="K77" s="1" t="s">
-        <v>134</v>
+      <c r="L77" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,13 +3227,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J78" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="K78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="K78" s="1" t="s">
-        <v>135</v>
+      <c r="L78" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,13 +3241,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J79" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="K79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="K79" s="1" t="s">
-        <v>31</v>
+      <c r="L79" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2323,13 +3255,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J80" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="K80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="K80" s="1" t="s">
-        <v>136</v>
+      <c r="L80" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>